<commit_message>
(U)    docs/ content added and updated
</commit_message>
<xml_diff>
--- a/docs/ISO 18000-6C Gen Notes.xlsx
+++ b/docs/ISO 18000-6C Gen Notes.xlsx
@@ -7,11 +7,11 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Commands" sheetId="1" r:id="rId1"/>
+    <sheet name="Misc." sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$N$58</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Commands!$A$1:$N$58</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -720,8 +720,8 @@
   </sheetPr>
   <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1399,7 +1399,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
(+)    <in prog> add Finite RFID Demo, structure in place        - switched to b0 TX first (BYTE_SWAP_EN=T)        - !!!?disabled Preamble        - sending jumk right now
</commit_message>
<xml_diff>
--- a/docs/ISO 18000-6C Gen Notes.xlsx
+++ b/docs/ISO 18000-6C Gen Notes.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Commands" sheetId="1" r:id="rId1"/>
-    <sheet name="Misc." sheetId="2" r:id="rId2"/>
+    <sheet name="Link Timing" sheetId="3" r:id="rId2"/>
+    <sheet name="Misc." sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Commands!$A$1:$N$58</definedName>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="144">
   <si>
     <t>Targets</t>
   </si>
@@ -371,13 +372,97 @@
   </si>
   <si>
     <t>counts</t>
+  </si>
+  <si>
+    <t>Tchip</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Nom</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>[1] Table 193 (p.153)</t>
+  </si>
+  <si>
+    <t>RTCal</t>
+  </si>
+  <si>
+    <t>TRCal</t>
+  </si>
+  <si>
+    <t>Data-0</t>
+  </si>
+  <si>
+    <t>Data-1</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>expected val</t>
+  </si>
+  <si>
+    <t>Tag Resp</t>
+  </si>
+  <si>
+    <t>not needed</t>
+  </si>
+  <si>
+    <t>(T1+T3)=T4</t>
+  </si>
+  <si>
+    <t>set to static val</t>
+  </si>
+  <si>
+    <t>Frame-Sync</t>
+  </si>
+  <si>
+    <t>Preamble</t>
+  </si>
+  <si>
+    <t>[1].9.3.1.2.8 (Fig 38)</t>
+  </si>
+  <si>
+    <t>N=61</t>
+  </si>
+  <si>
+    <t>N=22</t>
+  </si>
+  <si>
+    <t>Command Durations (Max, if all Data-1's)</t>
+  </si>
+  <si>
+    <t>R=&gt;T preamble and frame-sync</t>
+  </si>
+  <si>
+    <t>Buffer Calcs</t>
+  </si>
+  <si>
+    <t>#Bytes</t>
+  </si>
+  <si>
+    <t>#Chips</t>
+  </si>
+  <si>
+    <t>t_buff</t>
+  </si>
+  <si>
+    <t>ms</t>
+  </si>
+  <si>
+    <t>t_post</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -393,16 +478,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -410,11 +509,274 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -435,6 +797,70 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -720,8 +1146,8 @@
   </sheetPr>
   <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1396,6 +1822,360 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1">
+        <f>Commands!C11</f>
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1">
+        <f>1/(B2*1000)*1000000</f>
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <f>Commands!C13</f>
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F2">
+        <v>12.5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4">
+        <f>(Commands!C19+Commands!C18)</f>
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>121</v>
+      </c>
+      <c r="F4">
+        <f>(Commands!C21+Commands!C18)</f>
+        <v>75</v>
+      </c>
+      <c r="G4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5">
+        <f>(Commands!C20+Commands!C18)</f>
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>122</v>
+      </c>
+      <c r="F5">
+        <f>(Commands!C22+Commands!C18)</f>
+        <v>212.5</v>
+      </c>
+      <c r="G5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>127</v>
+      </c>
+      <c r="B7">
+        <f>16*F1</f>
+        <v>400</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="31" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B11" s="26">
+        <f>MAX(F4, 10*F1) - 2</f>
+        <v>248</v>
+      </c>
+      <c r="C11" s="21">
+        <f>MAX(F4, 10*F1)</f>
+        <v>250</v>
+      </c>
+      <c r="D11" s="29">
+        <f>MAX(F4, 10*F1) + 2</f>
+        <v>252</v>
+      </c>
+      <c r="E11" s="26">
+        <v>250</v>
+      </c>
+      <c r="F11" s="30" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12" s="27">
+        <f>3*F1</f>
+        <v>75</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="19">
+        <f>20*F1</f>
+        <v>500</v>
+      </c>
+      <c r="E12" s="27">
+        <v>75</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B13" s="27">
+        <v>0</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="27">
+        <f>E14-E11</f>
+        <v>475</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" s="28">
+        <f>2*F4</f>
+        <v>150</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="28">
+        <f>B7+E11+E12</f>
+        <v>725</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="15" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>131</v>
+      </c>
+      <c r="B18">
+        <f>Commands!C7+(Commands!C19+Commands!C18)+(Commands!C21+Commands!C18)</f>
+        <v>112.5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>132</v>
+      </c>
+      <c r="B19">
+        <f>B18+(Commands!C22+Commands!C18)</f>
+        <v>325</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21">
+        <f>B18+61*(Commands!C20+Commands!C18)</f>
+        <v>3162.5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22">
+        <f>B19+22*(Commands!C20+Commands!C18)</f>
+        <v>1425</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="31" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>139</v>
+      </c>
+      <c r="B25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>140</v>
+      </c>
+      <c r="B26">
+        <f>B25*8</f>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>141</v>
+      </c>
+      <c r="B28">
+        <f>B26*F2</f>
+        <v>10000</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <f>B28/1000</f>
+        <v>10</v>
+      </c>
+      <c r="C29" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>143</v>
+      </c>
+      <c r="B31">
+        <f>B28-E14-B21-E14-B22-E14</f>
+        <v>3237.5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
(C)    cleaned up file names ("\'") so project can now be Zipped
</commit_message>
<xml_diff>
--- a/docs/ISO 18000-6C Gen Notes.xlsx
+++ b/docs/ISO 18000-6C Gen Notes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Commands" sheetId="1" r:id="rId1"/>
-    <sheet name="Misc." sheetId="2" r:id="rId2"/>
+    <sheet name="Link Timing" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Commands!$A$1:$N$58</definedName>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="108">
   <si>
     <t>Targets</t>
   </si>
@@ -292,54 +292,12 @@
     <t>1000 0 00 1 00 11 1 0000</t>
   </si>
   <si>
-    <t>Query</t>
-  </si>
-  <si>
-    <t>22bits</t>
-  </si>
-  <si>
-    <t>Pre</t>
-  </si>
-  <si>
-    <t>Del+D0+RTCal+TRCal</t>
-  </si>
-  <si>
-    <t>tr</t>
-  </si>
-  <si>
-    <t>rt</t>
-  </si>
-  <si>
-    <t>d0</t>
-  </si>
-  <si>
-    <t>del</t>
-  </si>
-  <si>
-    <t>d1</t>
-  </si>
-  <si>
     <t>Tpri</t>
   </si>
   <si>
     <t>T2</t>
   </si>
   <si>
-    <t>Select</t>
-  </si>
-  <si>
-    <t>Vals</t>
-  </si>
-  <si>
-    <t>61bits</t>
-  </si>
-  <si>
-    <t>FS</t>
-  </si>
-  <si>
-    <t>Del+D0+RTCal</t>
-  </si>
-  <si>
     <t>T1</t>
   </si>
   <si>
@@ -349,28 +307,58 @@
     <t>T4</t>
   </si>
   <si>
-    <t>2*RTCal</t>
-  </si>
-  <si>
-    <t>Any</t>
-  </si>
-  <si>
-    <t>3*Tpri</t>
-  </si>
-  <si>
-    <t>20*Tpri</t>
-  </si>
-  <si>
-    <t>MAX(RTCal, 10*Tpri)</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>ns</t>
-  </si>
-  <si>
-    <t>counts</t>
+    <r>
+      <t xml:space="preserve">Core Parameters </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(linked)</t>
+    </r>
+  </si>
+  <si>
+    <t>Chip</t>
+  </si>
+  <si>
+    <t>Data-0</t>
+  </si>
+  <si>
+    <t>Data-1</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Nom</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>* see [1] Table 193 for description</t>
+  </si>
+  <si>
+    <t>RTCal</t>
+  </si>
+  <si>
+    <t>TRCal</t>
+  </si>
+  <si>
+    <t>#Chips</t>
+  </si>
+  <si>
+    <t>&lt;- See [1] 9.3.2.1.8 for def</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time </t>
+  </si>
+  <si>
+    <t>Tag Res[</t>
   </si>
 </sst>
 </file>
@@ -394,15 +382,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -410,11 +410,244 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -435,6 +668,70 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -720,8 +1017,8 @@
   </sheetPr>
   <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1396,256 +1693,304 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <f>Commands!C11</f>
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <f>B3/12.5</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <f>Commands!C13</f>
+        <v>40</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5">
+        <f>Commands!C10</f>
+        <v>12.5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D5:D15" si="0">B5/12.5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <f>Commands!C12</f>
+        <v>12.5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9">
+        <f>1/(B4*1000)*1000000</f>
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="C2">
-        <v>12.5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2">
-        <f>40000</f>
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3">
+      <c r="B11">
+        <f>(Commands!C19+Commands!C18)</f>
         <v>25</v>
       </c>
-      <c r="G3" t="s">
-        <v>98</v>
-      </c>
-      <c r="H3">
-        <f>1/H2</f>
-        <v>2.5000000000000001E-5</v>
-      </c>
-      <c r="I3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="C4">
-        <f>4*12.5</f>
+      <c r="B12">
+        <f>(Commands!C20+Commands!C18)</f>
         <v>50</v>
       </c>
-      <c r="H4">
-        <f>H3*1000000</f>
-        <v>25</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="C12" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C5">
-        <f>62.5+12.5</f>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B14">
+        <f>(B11+B12)</f>
         <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C6">
-        <f>212.5</f>
-        <v>212.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>91</v>
-      </c>
-      <c r="C8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C9">
-        <f>C2+C3+C5+C6</f>
-        <v>325</v>
-      </c>
-      <c r="D9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C11">
-        <f>C2+C3+C5</f>
-        <v>112.5</v>
-      </c>
-      <c r="D11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>89</v>
-      </c>
-      <c r="B13" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14">
-        <f>C9+22*C4</f>
-        <v>1425</v>
       </c>
       <c r="C14" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B15">
+        <f>B7/(B4*1000)*1000000</f>
+        <v>200</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="E15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B17">
+        <f>16*B9</f>
+        <v>400</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="D19" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="B19" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B20">
-        <f>C11+61*C4</f>
-        <v>3162.5</v>
-      </c>
-      <c r="C20" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H23">
-        <f>16000000</f>
-        <v>16000000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>105</v>
-      </c>
-      <c r="H24">
-        <f>1/H23</f>
-        <v>6.2499999999999997E-8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="H25">
-        <f>H24*1000000000</f>
-        <v>62.5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B26">
-        <f>MAX(C5,250)</f>
+      <c r="E19" s="28" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20" s="18">
+        <f>MAX(B14,10*$B$9)-2</f>
+        <v>248</v>
+      </c>
+      <c r="C20" s="19">
+        <f>MAX(B14,10*$B$9)</f>
         <v>250</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H27">
-        <v>100</v>
-      </c>
-      <c r="I27" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>99</v>
-      </c>
-      <c r="H28">
-        <f>H27*1000</f>
-        <v>100000</v>
-      </c>
-      <c r="I28" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="C29">
-        <f>3*H4</f>
+      <c r="D20" s="25">
+        <f>MAX(B14,10*$B$9)+2</f>
+        <v>252</v>
+      </c>
+      <c r="E20" s="29">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21" s="20">
+        <f>3*B9</f>
         <v>75</v>
       </c>
-      <c r="H29">
-        <f>H28/H25</f>
-        <v>1600</v>
-      </c>
-      <c r="I29" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="C30">
-        <f>20*H4</f>
+      <c r="C21" s="21"/>
+      <c r="D21" s="26">
+        <f>20*B9</f>
         <v>500</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="E21" s="30">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22" s="20">
+        <v>0</v>
+      </c>
+      <c r="C22" s="21"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="30">
+        <f>E20+E21+B17-E20</f>
+        <v>475</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" s="22">
+        <f>2*B14</f>
+        <v>150</v>
+      </c>
+      <c r="C23" s="23"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="31">
+        <f>E20+E21+B17</f>
+        <v>725</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="17" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B38">
-        <f>2*C5</f>
-        <v>150</v>
-      </c>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="9"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="9"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>